<commit_message>
hien so dong them/ cap nhat tu fjle excel
</commit_message>
<xml_diff>
--- a/export/inputDSNV.xlsx
+++ b/export/inputDSNV.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VAN NHUAN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JAVA_SGU_24-25\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252767F2-C9B0-4E36-86A0-39A6DBFA94A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184FA1CE-9B7E-41F0-850F-4678880583EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8256" yWindow="2616" windowWidth="14784" windowHeight="9624" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="14784" windowHeight="9624" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>SĐT</t>
   </si>
   <si>
-    <t>Lương</t>
-  </si>
-  <si>
     <t>NV001</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>091234444</t>
+  </si>
+  <si>
+    <t>Lương Tháng</t>
   </si>
 </sst>
 </file>
@@ -382,12 +382,13 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -404,21 +405,21 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="E2">
         <v>5000000</v>
@@ -426,16 +427,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E3">
         <v>6000000</v>

</xml_diff>